<commit_message>
Adds perihelion and v0 values to spreadsheet
</commit_message>
<xml_diff>
--- a/Assets/Datafiles/Spreadsheets/SolarSystemValues.xlsx
+++ b/Assets/Datafiles/Spreadsheets/SolarSystemValues.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Actual</t>
   </si>
@@ -28,6 +28,12 @@
     <t>aphelion (10^6 km)</t>
   </si>
   <si>
+    <t>perihelion (10^6 km)</t>
+  </si>
+  <si>
+    <t>v_0 = sqrt(GM/ R_p)</t>
+  </si>
+  <si>
     <t>Sun</t>
   </si>
   <si>
@@ -65,6 +71,12 @@
   </si>
   <si>
     <t>aphelion</t>
+  </si>
+  <si>
+    <t>perihelion</t>
+  </si>
+  <si>
+    <t>v inital</t>
   </si>
 </sst>
 </file>
@@ -102,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -116,6 +128,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -124,9 +139,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -348,7 +361,8 @@
     <col customWidth="1" min="3" max="3" width="10.75"/>
     <col customWidth="1" min="4" max="4" width="15.25"/>
     <col customWidth="1" min="5" max="5" width="15.13"/>
-    <col customWidth="1" min="7" max="7" width="14.88"/>
+    <col customWidth="1" min="6" max="6" width="16.13"/>
+    <col customWidth="1" min="7" max="7" width="17.0"/>
     <col customWidth="1" min="8" max="8" width="19.63"/>
     <col customWidth="1" min="9" max="9" width="14.5"/>
   </cols>
@@ -372,206 +386,250 @@
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="F3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5">
         <v>333000.0</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="5">
         <v>697700.0</v>
       </c>
       <c r="D4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="4">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5">
         <v>0.0553</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="7">
         <f>4879/2</f>
         <v>2439.5</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="5">
         <v>57.9</v>
       </c>
       <c r="E5" s="1">
         <v>69.8</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="F5" s="4">
+        <v>46.0</v>
+      </c>
+      <c r="G5" s="8">
+        <f t="shared" ref="G5:G12" si="1">SQRT(((6.67*10^(-11)) * (1.989*10^30))/(F5*10^9))</f>
+        <v>53703.35185</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="4">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5">
         <v>0.815</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="5">
         <f>12104/2</f>
         <v>6052</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="5">
         <v>108.2</v>
       </c>
       <c r="E6" s="1">
         <v>108.9</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="F6" s="4">
+        <v>107.5</v>
+      </c>
+      <c r="G6" s="8">
+        <f t="shared" si="1"/>
+        <v>35129.83228</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="4">
+        <v>10</v>
+      </c>
+      <c r="B7" s="5">
         <v>1.0</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="5">
         <f>12756/2</f>
         <v>6378</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="5">
         <v>149.6</v>
       </c>
       <c r="E7" s="1">
         <v>152.1</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="5"/>
+      <c r="F7" s="4">
+        <v>147.1</v>
+      </c>
+      <c r="G7" s="8">
+        <f t="shared" si="1"/>
+        <v>30031.28892</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="6"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="4">
+        <v>11</v>
+      </c>
+      <c r="B8" s="5">
         <v>0.107</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="5">
         <f>6792/2</f>
         <v>3396</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="5">
         <v>228.0</v>
       </c>
       <c r="E8" s="1">
         <v>249.3</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="5"/>
+      <c r="F8" s="4">
+        <v>206.7</v>
+      </c>
+      <c r="G8" s="8">
+        <f t="shared" si="1"/>
+        <v>25334.36774</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="6"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="4">
+        <v>12</v>
+      </c>
+      <c r="B9" s="5">
         <v>317.8</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="5">
         <f>142984/2</f>
         <v>71492</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="5">
         <v>778.5</v>
       </c>
       <c r="E9" s="1">
         <v>816.4</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="5"/>
+      <c r="F9" s="4">
+        <v>740.6</v>
+      </c>
+      <c r="G9" s="8">
+        <f t="shared" si="1"/>
+        <v>13384.07787</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="6"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="4">
+        <v>13</v>
+      </c>
+      <c r="B10" s="5">
         <v>95.2</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="5">
         <f>120536/2</f>
         <v>60268</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="5">
         <v>1432.0</v>
       </c>
       <c r="E10" s="1">
         <v>1506.5</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5"/>
+      <c r="F10" s="4">
+        <v>1357.6</v>
+      </c>
+      <c r="G10" s="8">
+        <f t="shared" si="1"/>
+        <v>9885.403339</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="4">
+        <v>14</v>
+      </c>
+      <c r="B11" s="5">
         <v>14.5</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="5">
         <f>51118/2</f>
         <v>25559</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="5">
         <v>2867.0</v>
       </c>
       <c r="E11" s="1">
         <v>3001.4</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="5"/>
+      <c r="F11" s="4">
+        <v>2732.7</v>
+      </c>
+      <c r="G11" s="8">
+        <f t="shared" si="1"/>
+        <v>6967.617963</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="6"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="4">
+        <v>15</v>
+      </c>
+      <c r="B12" s="5">
         <v>17.1</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="5">
         <f>49528/2</f>
         <v>24764</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="5">
         <v>4515.0</v>
       </c>
       <c r="E12" s="1">
         <v>4558.9</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="5"/>
+      <c r="F12" s="4">
+        <v>4471.1</v>
+      </c>
+      <c r="G12" s="8">
+        <f t="shared" si="1"/>
+        <v>5447.197437</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="6"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -588,177 +646,247 @@
       <c r="B17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>16</v>
+      <c r="C17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="4">
+        <v>7</v>
+      </c>
+      <c r="B18" s="5">
         <v>333000.0</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="6">
         <v>697.7</v>
       </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="4">
+        <v>8</v>
+      </c>
+      <c r="B19" s="5">
         <v>0.0553</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="6">
         <v>2.44</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="6">
         <v>579.0</v>
       </c>
-      <c r="E19" s="8">
-        <f t="shared" ref="E19:E26" si="1">E5 * 10</f>
+      <c r="E19" s="9">
+        <f t="shared" ref="E19:F19" si="2">E5 * 10</f>
         <v>698</v>
+      </c>
+      <c r="F19" s="9">
+        <f t="shared" si="2"/>
+        <v>460</v>
+      </c>
+      <c r="G19" s="9">
+        <f t="shared" ref="G19:G26" si="4">G5*10^-3</f>
+        <v>53.70335185</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="4">
+        <v>9</v>
+      </c>
+      <c r="B20" s="5">
         <v>0.815</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="6">
         <v>6.052</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="6">
         <v>1082.0</v>
       </c>
-      <c r="E20" s="8">
-        <f t="shared" si="1"/>
+      <c r="E20" s="9">
+        <f t="shared" ref="E20:F20" si="3">E6 * 10</f>
         <v>1089</v>
+      </c>
+      <c r="F20" s="9">
+        <f t="shared" si="3"/>
+        <v>1075</v>
+      </c>
+      <c r="G20" s="9">
+        <f t="shared" si="4"/>
+        <v>35.12983228</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="4">
+        <v>10</v>
+      </c>
+      <c r="B21" s="5">
         <v>1.0</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="5">
         <f>12756/2 *10^(-3)</f>
         <v>6.378</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="6">
         <v>1496.0</v>
       </c>
-      <c r="E21" s="8">
-        <f t="shared" si="1"/>
+      <c r="E21" s="9">
+        <f t="shared" ref="E21:F21" si="5">E7 * 10</f>
         <v>1521</v>
+      </c>
+      <c r="F21" s="9">
+        <f t="shared" si="5"/>
+        <v>1471</v>
+      </c>
+      <c r="G21" s="9">
+        <f t="shared" si="4"/>
+        <v>30.03128892</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="4">
+        <v>11</v>
+      </c>
+      <c r="B22" s="5">
         <v>0.107</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="5">
         <f>6792/2 *10^(-3)</f>
         <v>3.396</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="6">
         <v>2280.0</v>
       </c>
-      <c r="E22" s="8">
-        <f t="shared" si="1"/>
+      <c r="E22" s="9">
+        <f t="shared" ref="E22:F22" si="6">E8 * 10</f>
         <v>2493</v>
+      </c>
+      <c r="F22" s="9">
+        <f t="shared" si="6"/>
+        <v>2067</v>
+      </c>
+      <c r="G22" s="9">
+        <f t="shared" si="4"/>
+        <v>25.33436774</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="4">
+        <v>12</v>
+      </c>
+      <c r="B23" s="5">
         <v>317.8</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="5">
         <f>142984/2 *10^(-3)</f>
         <v>71.492</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="6">
         <v>7785.0</v>
       </c>
-      <c r="E23" s="8">
-        <f t="shared" si="1"/>
+      <c r="E23" s="9">
+        <f t="shared" ref="E23:F23" si="7">E9 * 10</f>
         <v>8164</v>
+      </c>
+      <c r="F23" s="9">
+        <f t="shared" si="7"/>
+        <v>7406</v>
+      </c>
+      <c r="G23" s="9">
+        <f t="shared" si="4"/>
+        <v>13.38407787</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="4">
+        <v>13</v>
+      </c>
+      <c r="B24" s="5">
         <v>95.2</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="5">
         <f>120536/2 *10^(-3)</f>
         <v>60.268</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="6">
         <v>14320.0</v>
       </c>
-      <c r="E24" s="8">
-        <f t="shared" si="1"/>
+      <c r="E24" s="9">
+        <f t="shared" ref="E24:F24" si="8">E10 * 10</f>
         <v>15065</v>
+      </c>
+      <c r="F24" s="9">
+        <f t="shared" si="8"/>
+        <v>13576</v>
+      </c>
+      <c r="G24" s="9">
+        <f t="shared" si="4"/>
+        <v>9.885403339</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="4">
+        <v>14</v>
+      </c>
+      <c r="B25" s="5">
         <v>14.5</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="5">
         <f>51118/2 *10^(-3)</f>
         <v>25.559</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="6">
         <v>28670.0</v>
       </c>
-      <c r="E25" s="8">
-        <f t="shared" si="1"/>
+      <c r="E25" s="9">
+        <f t="shared" ref="E25:F25" si="9">E11 * 10</f>
         <v>30014</v>
+      </c>
+      <c r="F25" s="9">
+        <f t="shared" si="9"/>
+        <v>27327</v>
+      </c>
+      <c r="G25" s="9">
+        <f t="shared" si="4"/>
+        <v>6.967617963</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="4">
+        <v>15</v>
+      </c>
+      <c r="B26" s="5">
         <v>17.1</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="5">
         <f>49528/2
  *10^(-3)</f>
         <v>24.764</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="6">
         <v>45150.0</v>
       </c>
-      <c r="E26" s="8">
-        <f t="shared" si="1"/>
+      <c r="E26" s="9">
+        <f t="shared" ref="E26:F26" si="10">E12 * 10</f>
         <v>45589</v>
+      </c>
+      <c r="F26" s="9">
+        <f t="shared" si="10"/>
+        <v>44711</v>
+      </c>
+      <c r="G26" s="9">
+        <f t="shared" si="4"/>
+        <v>5.447197437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>